<commit_message>
Updation in Week 45
</commit_message>
<xml_diff>
--- a/Week 45/vishnu_2.xlsx
+++ b/Week 45/vishnu_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Milestone Toolkit\vishnu\Weekly Report\Nov\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Support Analysis\Week 45\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3216,8 +3216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,8 +3425,8 @@
       <c r="B17" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="38" t="s">
-        <v>17</v>
+      <c r="C17" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="D17" s="29">
         <v>0.8</v>

</xml_diff>